<commit_message>
se realiza escenario de indisponibilidad, se actualzian evidencias y metricas de la infraestructura
</commit_message>
<xml_diff>
--- a/Documento evaluación No Funcional.xlsx
+++ b/Documento evaluación No Funcional.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejandra.ospina\Documents\GitHub\testing-performance-puntos-colombia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8097267-D1CE-45D2-B456-5C4482619277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6173EF0D-8545-4D36-8418-0DE9352C4E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{06B755A2-69F7-43B0-8376-5061E54A97FE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{06B755A2-69F7-43B0-8376-5061E54A97FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Ejecuciones" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>Prueba</t>
   </si>
@@ -134,7 +134,39 @@
     <t>Escenario 2 Fase 2</t>
   </si>
   <si>
-    <t>Producción</t>
+    <t>Producción Fase 3</t>
+  </si>
+  <si>
+    <t>Escenario indisponibilidad</t>
+  </si>
+  <si>
+    <t>indisponibilidad</t>
+  </si>
+  <si>
+    <t>Re iniciando el micro</t>
+  </si>
+  <si>
+    <t>Cambiando la parametrización de los hilos de 10 a 1 (como está actualmente en producción)</t>
+  </si>
+  <si>
+    <t>10
+1
+10</t>
+  </si>
+  <si>
+    <t>Durante la ejecución completa</t>
+  </si>
+  <si>
+    <t>Desde los re inicios del micro</t>
+  </si>
+  <si>
+    <t>Colas:</t>
+  </si>
+  <si>
+    <t>Después</t>
+  </si>
+  <si>
+    <t>Se procesaron todos los registros nuevos en bd, los demás en el log se ven como duplicados</t>
   </si>
 </sst>
 </file>
@@ -143,9 +175,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="174" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,19 +200,13 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -190,6 +216,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -267,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -292,86 +324,81 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -401,9 +428,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>449518</xdr:colOff>
+      <xdr:colOff>446343</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>28181</xdr:rowOff>
+      <xdr:rowOff>31356</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -445,7 +472,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>311423</xdr:colOff>
+      <xdr:colOff>314598</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>171114</xdr:rowOff>
     </xdr:to>
@@ -491,7 +518,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>111125</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>88052</xdr:rowOff>
+      <xdr:rowOff>84877</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -621,9 +648,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>26381</xdr:colOff>
+      <xdr:colOff>29556</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>123380</xdr:rowOff>
+      <xdr:rowOff>126555</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -648,6 +675,1156 @@
         <a:xfrm>
           <a:off x="4524375" y="6515100"/>
           <a:ext cx="17552381" cy="3561905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>18321</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>540975</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>171528</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6EE5AA0-5029-989C-3240-375D33BBB234}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="10857114"/>
+          <a:ext cx="5840378" cy="1959672"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>152256</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>316872</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>130716</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA156B9F-B126-73BD-8685-8C9383628F23}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="15326566"/>
+          <a:ext cx="4846283" cy="1423633"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>41987</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>166942</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>8977</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>48488</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Imagen 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4079C5A-D7ED-AFFC-CDD0-23FA278C7309}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="41987" y="12992847"/>
+          <a:ext cx="3742284" cy="1146072"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>104318</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>390284</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>83786</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Imagen 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3268F0E-BBA1-4B4D-13B0-4069185EB852}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="16904447"/>
+          <a:ext cx="4162403" cy="885876"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>208436</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>119487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>505521</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>30601</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Imagen 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03E3BFE2-6F51-A543-E9D7-5F149A9D5942}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="208436" y="14390565"/>
+          <a:ext cx="1771927" cy="817521"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>7281</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>173956</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>656358</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>39163</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Imagen 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9D0100B-D84B-49D7-AB08-8FABED9F931A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7281" y="18057965"/>
+          <a:ext cx="5184838" cy="2394259"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>4088</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>312851</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>65434</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Imagen 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4B50A1E-7730-1359-8124-C6D84A357E15}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="23668786"/>
+          <a:ext cx="8663648" cy="2416101"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>7960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>516420</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>67951</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Imagen 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB904A96-99E3-8CC0-9407-30C26B51A223}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="26201710"/>
+          <a:ext cx="5049006" cy="2411571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>142832</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>351636</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>114546</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Imagen 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA947D3A-2CB4-EE04-BA63-274E86E6CD32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="28684987"/>
+          <a:ext cx="6414682" cy="2862059"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>7282</xdr:colOff>
+      <xdr:row>175</xdr:row>
+      <xdr:rowOff>166199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>609810</xdr:colOff>
+      <xdr:row>185</xdr:row>
+      <xdr:rowOff>25667</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Imagen 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01525D7B-AEA1-B258-800E-1A1D7227808B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7282" y="31779346"/>
+          <a:ext cx="5898756" cy="1669108"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>186</xdr:row>
+      <xdr:rowOff>175468</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>47461</xdr:colOff>
+      <xdr:row>197</xdr:row>
+      <xdr:rowOff>133198</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Imagen 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D9C75C3-837F-E9F1-8941-3A989231589B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="36304778"/>
+          <a:ext cx="4576872" cy="1944842"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>198</xdr:row>
+      <xdr:rowOff>147802</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>496980</xdr:colOff>
+      <xdr:row>206</xdr:row>
+      <xdr:rowOff>174226</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Imagen 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54AAE2AD-561B-2854-C676-884E06A57884}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="38444871"/>
+          <a:ext cx="5029566" cy="1471597"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>10073</xdr:colOff>
+      <xdr:row>207</xdr:row>
+      <xdr:rowOff>167694</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>540474</xdr:colOff>
+      <xdr:row>220</xdr:row>
+      <xdr:rowOff>161910</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Imagen 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0CF5803-551C-69AD-59F6-D3BFAEDC4BFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10073" y="40090582"/>
+          <a:ext cx="5066162" cy="2339446"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>223</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>212506</xdr:colOff>
+      <xdr:row>230</xdr:row>
+      <xdr:rowOff>54362</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Imagen 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69EDC670-751B-1C75-AD37-01C156F0E0D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="46017187"/>
+          <a:ext cx="1690523" cy="1322063"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>271</xdr:row>
+      <xdr:rowOff>19449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>960</xdr:colOff>
+      <xdr:row>281</xdr:row>
+      <xdr:rowOff>59684</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Imagen 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F6CBDFB-FE9E-632F-7278-CBDAB7028397}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="54755354"/>
+          <a:ext cx="6822831" cy="1846700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>58278</xdr:colOff>
+      <xdr:row>282</xdr:row>
+      <xdr:rowOff>171505</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>77279</xdr:colOff>
+      <xdr:row>296</xdr:row>
+      <xdr:rowOff>29742</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Imagen 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3BDFCF8-2DBB-7056-7018-B8773ED9133F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="58278" y="56894522"/>
+          <a:ext cx="3787945" cy="2384113"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>297</xdr:row>
+      <xdr:rowOff>7479</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>57380</xdr:colOff>
+      <xdr:row>307</xdr:row>
+      <xdr:rowOff>49930</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Imagen 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D27915A-FC4A-6B32-315B-F1060D841075}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="59440195"/>
+          <a:ext cx="4589966" cy="1852091"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>308</xdr:row>
+      <xdr:rowOff>7366</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>754022</xdr:colOff>
+      <xdr:row>316</xdr:row>
+      <xdr:rowOff>142265</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="Imagen 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21822A61-C285-0656-8724-EBE8407A8BEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="61427194"/>
+          <a:ext cx="3762499" cy="1583246"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>20528</xdr:colOff>
+      <xdr:row>318</xdr:row>
+      <xdr:rowOff>3568</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1687</xdr:colOff>
+      <xdr:row>324</xdr:row>
+      <xdr:rowOff>142051</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Imagen 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC3A4CAB-7D4A-414E-4AC0-2C25215A643F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20528" y="63229861"/>
+          <a:ext cx="3750103" cy="1225538"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>585</xdr:colOff>
+      <xdr:row>326</xdr:row>
+      <xdr:rowOff>94428</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>526337</xdr:colOff>
+      <xdr:row>336</xdr:row>
+      <xdr:rowOff>87921</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Imagen 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA4570CD-6773-74AB-D569-E96D4DEF8602}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="585" y="64765894"/>
+          <a:ext cx="4291521" cy="1796783"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>337</xdr:row>
+      <xdr:rowOff>3175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>543920</xdr:colOff>
+      <xdr:row>347</xdr:row>
+      <xdr:rowOff>140067</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Imagen 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E3AB4FB-BAB5-94D4-1EE7-3AC098DE6F21}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="66661753"/>
+          <a:ext cx="5836973" cy="1946532"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>51771</xdr:colOff>
+      <xdr:row>348</xdr:row>
+      <xdr:rowOff>159187</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>336039</xdr:colOff>
+      <xdr:row>354</xdr:row>
+      <xdr:rowOff>7738</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Imagen 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F20D4A6B-E1F3-5B3D-5B69-9994468648AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="51771" y="68804877"/>
+          <a:ext cx="3292745" cy="935605"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>46093</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>495775</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>26527</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Imagen 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A130A1C2-C965-0E2B-4F62-641B4E560DE3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="17930102"/>
+          <a:ext cx="4264719" cy="2512660"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>356</xdr:row>
+      <xdr:rowOff>143697</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>347867</xdr:colOff>
+      <xdr:row>372</xdr:row>
+      <xdr:rowOff>117451</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="Imagen 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E0F0602-380C-5B43-DA78-CA186B84604D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="64453869"/>
+          <a:ext cx="4880453" cy="2864099"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>231</xdr:row>
+      <xdr:rowOff>100799</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>617129</xdr:colOff>
+      <xdr:row>249</xdr:row>
+      <xdr:rowOff>85287</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Imagen 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{936A1912-7EC4-DF1B-570D-30576DBAC6A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="41830152"/>
+          <a:ext cx="4386073" cy="3236126"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>29670</xdr:colOff>
+      <xdr:row>252</xdr:row>
+      <xdr:rowOff>135485</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>68086</xdr:colOff>
+      <xdr:row>267</xdr:row>
+      <xdr:rowOff>139591</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="Imagen 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67E53720-A63C-5176-CABB-3C18E51CDD2F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="29670" y="45658416"/>
+          <a:ext cx="4571002" cy="2713804"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -990,22 +2167,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50403015-8103-4ED3-9731-9EC8E56CD7CA}">
-  <dimension ref="A1:DOW16"/>
+  <dimension ref="A1:DOW15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.90625" customWidth="1"/>
     <col min="2" max="2" width="17.90625" style="1" customWidth="1"/>
-    <col min="3" max="5" width="9.90625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6328125" style="1" customWidth="1"/>
-    <col min="7" max="14" width="18.90625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="15.36328125" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="15.36328125" style="1" customWidth="1"/>
+    <col min="8" max="14" width="18.90625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14 3117:3117" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14 3117:3117" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1074,24 +2252,24 @@
       <c r="H2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="23">
+      <c r="I2" s="17">
         <f>(E2-D2)*1440</f>
         <v>150.99999999999994</v>
       </c>
-      <c r="J2" s="24">
+      <c r="J2" s="18">
         <f>I2/60</f>
         <v>2.5166666666666657</v>
       </c>
-      <c r="K2" s="25">
+      <c r="K2" s="19">
         <v>0.38334000000000001</v>
       </c>
-      <c r="L2" s="25">
+      <c r="L2" s="19">
         <v>3.0667</v>
       </c>
-      <c r="M2" s="25">
+      <c r="M2" s="19">
         <v>4.8933</v>
       </c>
-      <c r="N2" s="25">
+      <c r="N2" s="19">
         <v>54.77</v>
       </c>
     </row>
@@ -1125,7 +2303,7 @@
         <f>(E3-D3)*1440</f>
         <v>23.999999999999993</v>
       </c>
-      <c r="J3" s="16">
+      <c r="J3" s="14">
         <f>I3/60</f>
         <v>0.39999999999999986</v>
       </c>
@@ -1173,31 +2351,31 @@
         <f>(E4-D4)*1440</f>
         <v>185.05000000000015</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="14">
         <f>I4/60</f>
         <v>3.0841666666666692</v>
       </c>
-      <c r="K4" s="32">
+      <c r="K4" s="3">
         <v>7.6890999999999998</v>
       </c>
-      <c r="L4" s="32">
+      <c r="L4" s="3">
         <v>30.036000000000001</v>
       </c>
-      <c r="M4" s="32">
+      <c r="M4" s="3">
         <v>4.8239999999999998</v>
       </c>
-      <c r="N4" s="32">
+      <c r="N4" s="3">
         <v>36.909999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:14 3117:3117" x14ac:dyDescent="0.35">
-      <c r="A5" s="17">
+      <c r="A5" s="15">
         <v>45593</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="24">
         <v>41757</v>
       </c>
       <c r="D5" s="9">
@@ -1209,23 +2387,23 @@
       <c r="F5" s="26">
         <v>4</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="28">
         <f>(C5*I2)/C2</f>
         <v>600.5054285714283</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="22">
         <f>G5/60</f>
         <v>10.008423809523805</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I5" s="28">
         <f>((E5-D5)+(E6-D6))*1440</f>
         <v>388.99999999999983</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="23">
         <f>I5/60</f>
         <v>6.4833333333333307</v>
       </c>
-      <c r="K5" s="28">
+      <c r="K5" s="21">
         <v>7.1299000000000001</v>
       </c>
       <c r="L5" s="3">
@@ -1242,8 +2420,8 @@
       <c r="A6" s="4">
         <v>45594</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
       <c r="D6" s="9">
         <v>0.29166666666666669</v>
       </c>
@@ -1251,10 +2429,10 @@
         <v>0.44374999999999998</v>
       </c>
       <c r="F6" s="27"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="19"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="23"/>
       <c r="K6" s="3">
         <v>1.1598999999999999</v>
       </c>
@@ -1275,7 +2453,7 @@
       <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="12">
         <v>62243</v>
       </c>
       <c r="D7" s="9">
@@ -1299,7 +2477,7 @@
         <f>(E7-D7)*1440</f>
         <v>393.99999999999994</v>
       </c>
-      <c r="J7" s="16">
+      <c r="J7" s="14">
         <f>I7/60</f>
         <v>6.5666666666666655</v>
       </c>
@@ -1323,7 +2501,7 @@
       <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="12">
         <v>21760</v>
       </c>
       <c r="D8" s="9">
@@ -1333,7 +2511,7 @@
         <v>0.76930555555555558</v>
       </c>
       <c r="F8" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G8" s="6">
         <f>((C8*I3)/C3)</f>
@@ -1347,7 +2525,7 @@
         <f>(E8-D8)*1440</f>
         <v>139.79999999999995</v>
       </c>
-      <c r="J8" s="16">
+      <c r="J8" s="14">
         <f>I8/60</f>
         <v>2.3299999999999992</v>
       </c>
@@ -1364,12 +2542,12 @@
         <v>38.636000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:14 3117:3117" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14 3117:3117" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="12">
         <v>10933</v>
       </c>
       <c r="D9" s="9">
@@ -1382,18 +2560,19 @@
         <v>10</v>
       </c>
       <c r="G9" s="6">
-        <v>80</v>
+        <f t="shared" ref="G9:G11" si="0">((C9*I4)/C4)</f>
+        <v>67.90238798456123</v>
       </c>
       <c r="H9" s="8">
         <f>G9/60</f>
-        <v>1.3333333333333333</v>
+        <v>1.1317064664093539</v>
       </c>
       <c r="I9" s="6">
-        <f>(E9-D9)*1440</f>
+        <f t="shared" ref="I9:I11" si="1">(E9-D9)*1440</f>
         <v>55.299999999999855</v>
       </c>
-      <c r="J9" s="16">
-        <f>I9/60</f>
+      <c r="J9" s="14">
+        <f t="shared" ref="J9:J11" si="2">I9/60</f>
         <v>0.9216666666666643</v>
       </c>
       <c r="K9" s="3">
@@ -1409,81 +2588,91 @@
         <v>37.997999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:14 3117:3117" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="31"/>
+    <row r="10" spans="1:14 3117:3117" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1500000</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="20">
+        <v>10</v>
+      </c>
+      <c r="G10" s="32">
+        <f t="shared" si="0"/>
+        <v>13973.70500754364</v>
+      </c>
+      <c r="H10" s="32">
+        <f>G10/60</f>
+        <v>232.89508345906066</v>
+      </c>
+      <c r="I10" s="32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="31"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10"/>
+      <c r="DOW10" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="11" spans="1:14 3117:3117" x14ac:dyDescent="0.35">
-      <c r="B11" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1500000</v>
-      </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="2">
-        <v>10</v>
-      </c>
-      <c r="G11" s="6">
-        <f>((C11*I9)/C9)</f>
-        <v>7587.1215585840828</v>
-      </c>
-      <c r="H11" s="6">
-        <f>G11/60</f>
-        <v>126.45202597640137</v>
-      </c>
-      <c r="I11" s="6"/>
+    <row r="11" spans="1:14 3117:3117" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="34">
+        <v>45601</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="3">
+        <v>11005</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0.38819444444444445</v>
+      </c>
+      <c r="E11" s="9">
+        <v>0.44108796296296299</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6">
+        <f>(E11-D11)*1440</f>
+        <v>76.166666666666686</v>
+      </c>
       <c r="J11" s="14">
-        <f>I11/60</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="10"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11"/>
-      <c r="DOW11" t="s">
-        <v>9</v>
+        <f t="shared" si="2"/>
+        <v>1.2694444444444448</v>
+      </c>
+      <c r="K11" s="3">
+        <v>25.588000000000001</v>
+      </c>
+      <c r="L11" s="30">
+        <v>99.951999999999998</v>
+      </c>
+      <c r="M11" s="3">
+        <v>4.8255999999999997</v>
+      </c>
+      <c r="N11" s="35">
+        <v>36.921999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:14 3117:3117" x14ac:dyDescent="0.35">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12"/>
+    <row r="13" spans="1:14 3117:3117" x14ac:dyDescent="0.35">
+      <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:14 3117:3117" x14ac:dyDescent="0.35">
-      <c r="G14" s="11"/>
-      <c r="H14" s="33">
-        <f>H11/24</f>
-        <v>5.2688344156833908</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14 3117:3117" x14ac:dyDescent="0.35">
-      <c r="C16" s="7"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="15"/>
+    <row r="15" spans="1:14 3117:3117" x14ac:dyDescent="0.35">
+      <c r="C15" s="7"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1495,7 +2684,7 @@
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="G5:G6"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -1504,10 +2693,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F41588-B940-490C-BA03-A9DB924B9B82}">
-  <dimension ref="A1:A36"/>
+  <dimension ref="A1:C356"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="232" zoomScaleNormal="232" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A235" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C224" sqref="C224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1535,8 +2724,48 @@
         <v>18</v>
       </c>
     </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="224" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C224" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A232" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A252" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A271" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A356" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
actualización del documento de evaluación no funcional con monitoreo en producción
</commit_message>
<xml_diff>
--- a/Documento evaluación No Funcional.xlsx
+++ b/Documento evaluación No Funcional.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejandra.ospina\Documents\GitHub\testing-performance-puntos-colombia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6173EF0D-8545-4D36-8418-0DE9352C4E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38877EB7-B397-4C51-9132-FD080BA9EC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{06B755A2-69F7-43B0-8376-5061E54A97FE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{06B755A2-69F7-43B0-8376-5061E54A97FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Ejecuciones" sheetId="1" r:id="rId1"/>
     <sheet name="Evidencias" sheetId="2" r:id="rId2"/>
+    <sheet name="Producción" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,6 +41,9 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={A9AE1795-81AE-40CA-8344-5507ACF91599}</author>
+    <author>tc={363ECD93-26FB-468A-A3FC-79E342B3F699}</author>
+    <author>tc={A2B3B1FA-E3C8-4D12-A0C1-5FB22B1DCE15}</author>
+    <author>tc={CD0C63BA-84AD-4E0F-9FE4-DDEA21172978}</author>
   </authors>
   <commentList>
     <comment ref="N2" authorId="0" shapeId="0" xr:uid="{A9AE1795-81AE-40CA-8344-5507ACF91599}">
@@ -50,12 +54,84 @@
     No se había desactivado el envío a puntos Colombia y el microservicio no tenía las capacidades de producción</t>
       </text>
     </comment>
+    <comment ref="C12" authorId="1" shapeId="0" xr:uid="{363ECD93-26FB-468A-A3FC-79E342B3F699}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Cantidad procesada 5397 por cuello de botella en CPU de bd</t>
+      </text>
+    </comment>
+    <comment ref="C13" authorId="2" shapeId="0" xr:uid="{A2B3B1FA-E3C8-4D12-A0C1-5FB22B1DCE15}">
+      <text>
+        <t xml:space="preserve">[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    2785 también alcanzó max de 90% de CPU
+</t>
+      </text>
+    </comment>
+    <comment ref="C15" authorId="3" shapeId="0" xr:uid="{CD0C63BA-84AD-4E0F-9FE4-DDEA21172978}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    despues del indice</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={FC007BD5-3994-4C6C-BA6A-22C747B225A9}</author>
+    <author>tc={8589356F-B85D-48F5-9A30-671E3104710B}</author>
+    <author>tc={BBA738C8-4A2B-4546-8729-695DBFD78E1C}</author>
+    <author>tc={FB9D1AF4-0648-4174-BCCD-8D55D0C349C2}</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{FC007BD5-3994-4C6C-BA6A-22C747B225A9}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Cantidad procesada 5397 por cuello de botella en CPU de bd</t>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="1" shapeId="0" xr:uid="{8589356F-B85D-48F5-9A30-671E3104710B}">
+      <text>
+        <t xml:space="preserve">[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    2785 también alcanzó max de 90% de CPU
+</t>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="2" shapeId="0" xr:uid="{BBA738C8-4A2B-4546-8729-695DBFD78E1C}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    despues del indice</t>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="3" shapeId="0" xr:uid="{FB9D1AF4-0648-4174-BCCD-8D55D0C349C2}">
+      <text>
+        <t xml:space="preserve">[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Aumentó después de proceso de sincronización 
+</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
   <si>
     <t>Prueba</t>
   </si>
@@ -132,9 +208,6 @@
   </si>
   <si>
     <t>Escenario 2 Fase 2</t>
-  </si>
-  <si>
-    <t>Producción Fase 3</t>
   </si>
   <si>
     <t>Escenario indisponibilidad</t>
@@ -167,6 +240,51 @@
   </si>
   <si>
     <t>Se procesaron todos los registros nuevos en bd, los demás en el log se ven como duplicados</t>
+  </si>
+  <si>
+    <t>Estimacion Producción Fase 3</t>
+  </si>
+  <si>
+    <t>Producción Ejecución</t>
+  </si>
+  <si>
+    <t>Cantidad registros procesados en 13 horas con 8 hilos y un minuto de frecuencia</t>
+  </si>
+  <si>
+    <t>5-6/11/2024</t>
+  </si>
+  <si>
+    <t>Días con frecuencia de 1 min</t>
+  </si>
+  <si>
+    <t>Cantidad registros procesados en 1 horas con 8 hilos y 30 seg de frecuencia</t>
+  </si>
+  <si>
+    <t>Días con frecuencia de 30 seg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Despues de la sincronización de las 11 aumentó </t>
+  </si>
+  <si>
+    <t>estado Actual en colas</t>
+  </si>
+  <si>
+    <t>Escenario</t>
+  </si>
+  <si>
+    <t>Cantidad actual registros en cola</t>
+  </si>
+  <si>
+    <t>Cantidad actual registros procesados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06/11/2024 Despues de la sincronización de las 11 aumentó </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Días con 8 hilos con frecuencia de 1 min </t>
+  </si>
+  <si>
+    <t>Díascon 8 hilos con frecuencia de 30 seg</t>
   </si>
 </sst>
 </file>
@@ -194,19 +312,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="7"/>
-      <color rgb="FF16191F"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,6 +340,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -299,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -317,16 +441,12 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -360,6 +480,19 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -381,23 +514,43 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2162,24 +2315,53 @@
   <threadedComment ref="N2" dT="2024-10-30T13:08:41.44" personId="{4E0D853E-4229-4B54-9F3B-11917A4E58D5}" id="{A9AE1795-81AE-40CA-8344-5507ACF91599}">
     <text>No se había desactivado el envío a puntos Colombia y el microservicio no tenía las capacidades de producción</text>
   </threadedComment>
+  <threadedComment ref="C12" dT="2024-11-05T20:33:55.08" personId="{4E0D853E-4229-4B54-9F3B-11917A4E58D5}" id="{363ECD93-26FB-468A-A3FC-79E342B3F699}">
+    <text>Cantidad procesada 5397 por cuello de botella en CPU de bd</text>
+  </threadedComment>
+  <threadedComment ref="C13" dT="2024-11-05T21:34:37.25" personId="{4E0D853E-4229-4B54-9F3B-11917A4E58D5}" id="{A2B3B1FA-E3C8-4D12-A0C1-5FB22B1DCE15}">
+    <text xml:space="preserve">2785 también alcanzó max de 90% de CPU
+</text>
+  </threadedComment>
+  <threadedComment ref="C15" dT="2024-11-05T22:40:35.23" personId="{4E0D853E-4229-4B54-9F3B-11917A4E58D5}" id="{CD0C63BA-84AD-4E0F-9FE4-DDEA21172978}">
+    <text>despues del indice</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B2" dT="2024-11-05T20:33:55.08" personId="{4E0D853E-4229-4B54-9F3B-11917A4E58D5}" id="{FC007BD5-3994-4C6C-BA6A-22C747B225A9}">
+    <text>Cantidad procesada 5397 por cuello de botella en CPU de bd</text>
+  </threadedComment>
+  <threadedComment ref="B3" dT="2024-11-05T21:34:37.25" personId="{4E0D853E-4229-4B54-9F3B-11917A4E58D5}" id="{8589356F-B85D-48F5-9A30-671E3104710B}">
+    <text xml:space="preserve">2785 también alcanzó max de 90% de CPU
+</text>
+  </threadedComment>
+  <threadedComment ref="B5" dT="2024-11-05T22:40:35.23" personId="{4E0D853E-4229-4B54-9F3B-11917A4E58D5}" id="{BBA738C8-4A2B-4546-8729-695DBFD78E1C}">
+    <text>despues del indice</text>
+  </threadedComment>
+  <threadedComment ref="B9" dT="2024-11-06T21:59:37.34" personId="{4E0D853E-4229-4B54-9F3B-11917A4E58D5}" id="{FB9D1AF4-0648-4174-BCCD-8D55D0C349C2}">
+    <text xml:space="preserve">Aumentó después de proceso de sincronización 
+</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50403015-8103-4ED3-9731-9EC8E56CD7CA}">
-  <dimension ref="A1:DOW15"/>
+  <dimension ref="A1:DOW24"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView topLeftCell="B1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.90625" customWidth="1"/>
-    <col min="2" max="2" width="17.90625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.36328125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="15.36328125" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="7" width="15.36328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.81640625" style="1" customWidth="1"/>
+    <col min="3" max="5" width="15.36328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.36328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.81640625" style="1" customWidth="1"/>
     <col min="8" max="14" width="18.90625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2227,7 +2409,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14 3117:3117" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14 3117:3117" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>45589</v>
       </c>
@@ -2237,43 +2419,43 @@
       <c r="C2" s="3">
         <v>10500</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>0.75</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>0.85486111111111107</v>
       </c>
       <c r="F2" s="2">
         <v>4</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="17">
+      <c r="I2" s="15">
         <f>(E2-D2)*1440</f>
         <v>150.99999999999994</v>
       </c>
-      <c r="J2" s="18">
+      <c r="J2" s="16">
         <f>I2/60</f>
         <v>2.5166666666666657</v>
       </c>
-      <c r="K2" s="19">
+      <c r="K2" s="17">
         <v>0.38334000000000001</v>
       </c>
-      <c r="L2" s="19">
+      <c r="L2" s="17">
         <v>3.0667</v>
       </c>
-      <c r="M2" s="19">
+      <c r="M2" s="17">
         <v>4.8933</v>
       </c>
-      <c r="N2" s="19">
+      <c r="N2" s="17">
         <v>54.77</v>
       </c>
     </row>
-    <row r="3" spans="1:14 3117:3117" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14 3117:3117" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>45595</v>
       </c>
@@ -2284,26 +2466,26 @@
         <f>10962-7625</f>
         <v>3337</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>0.46944444444444444</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>0.4861111111111111</v>
       </c>
       <c r="F3" s="2">
         <v>8</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="8" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="3">
         <f>(E3-D3)*1440</f>
         <v>23.999999999999993</v>
       </c>
-      <c r="J3" s="14">
+      <c r="J3" s="12">
         <f>I3/60</f>
         <v>0.39999999999999986</v>
       </c>
@@ -2320,7 +2502,7 @@
         <v>34.555</v>
       </c>
     </row>
-    <row r="4" spans="1:14 3117:3117" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14 3117:3117" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>45595</v>
       </c>
@@ -2330,10 +2512,10 @@
       <c r="C4" s="1">
         <v>29795</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>0.51315972222222217</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>0.64166666666666672</v>
       </c>
       <c r="F4" s="2">
@@ -2343,7 +2525,7 @@
         <f>(C4*I3)/C3</f>
         <v>214.28828288882224</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="7">
         <f>G4/60</f>
         <v>3.5714713814803707</v>
       </c>
@@ -2351,7 +2533,7 @@
         <f>(E4-D4)*1440</f>
         <v>185.05000000000015</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="12">
         <f>I4/60</f>
         <v>3.0841666666666692</v>
       </c>
@@ -2368,42 +2550,42 @@
         <v>36.909999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:14 3117:3117" x14ac:dyDescent="0.35">
-      <c r="A5" s="15">
+    <row r="5" spans="1:14 3117:3117" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="13">
         <v>45593</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="27">
         <v>41757</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>0.67361111111111116</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>0.79166666666666663</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="29">
         <v>4</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="31">
         <f>(C5*I2)/C2</f>
         <v>600.5054285714283</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="25">
         <f>G5/60</f>
         <v>10.008423809523805</v>
       </c>
-      <c r="I5" s="28">
+      <c r="I5" s="31">
         <f>((E5-D5)+(E6-D6))*1440</f>
         <v>388.99999999999983</v>
       </c>
-      <c r="J5" s="23">
+      <c r="J5" s="26">
         <f>I5/60</f>
         <v>6.4833333333333307</v>
       </c>
-      <c r="K5" s="21">
+      <c r="K5" s="19">
         <v>7.1299000000000001</v>
       </c>
       <c r="L5" s="3">
@@ -2416,23 +2598,23 @@
         <v>35.076999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:14 3117:3117" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14 3117:3117" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>45594</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="9">
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="8">
         <v>0.29166666666666669</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>0.44374999999999998</v>
       </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="23"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="26"/>
       <c r="K6" s="3">
         <v>1.1598999999999999</v>
       </c>
@@ -2453,13 +2635,13 @@
       <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="10">
         <v>62243</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>0.4548611111111111</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>0.72847222222222219</v>
       </c>
       <c r="F7" s="2">
@@ -2469,7 +2651,7 @@
         <f>((C7*I3)/C3)</f>
         <v>447.65717710518413</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="7">
         <f>G7/60</f>
         <v>7.4609529517530691</v>
       </c>
@@ -2477,7 +2659,7 @@
         <f>(E7-D7)*1440</f>
         <v>393.99999999999994</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="12">
         <f>I7/60</f>
         <v>6.5666666666666655</v>
       </c>
@@ -2501,13 +2683,13 @@
       <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="10">
         <v>21760</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>0.67222222222222228</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <v>0.76930555555555558</v>
       </c>
       <c r="F8" s="2">
@@ -2517,7 +2699,7 @@
         <f>((C8*I3)/C3)</f>
         <v>156.49985016481864</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="7">
         <f>G8/60</f>
         <v>2.6083308360803108</v>
       </c>
@@ -2525,7 +2707,7 @@
         <f>(E8-D8)*1440</f>
         <v>139.79999999999995</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="12">
         <f>I8/60</f>
         <v>2.3299999999999992</v>
       </c>
@@ -2542,37 +2724,37 @@
         <v>38.636000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:14 3117:3117" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14 3117:3117" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="10">
         <v>10933</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>0.68927083333333339</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>0.72767361111111106</v>
       </c>
       <c r="F9" s="2">
         <v>10</v>
       </c>
       <c r="G9" s="6">
-        <f t="shared" ref="G9:G11" si="0">((C9*I4)/C4)</f>
+        <f t="shared" ref="G9" si="0">((C9*I4)/C4)</f>
         <v>67.90238798456123</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <f>G9/60</f>
         <v>1.1317064664093539</v>
       </c>
       <c r="I9" s="6">
-        <f t="shared" ref="I9:I11" si="1">(E9-D9)*1440</f>
+        <f t="shared" ref="I9" si="1">(E9-D9)*1440</f>
         <v>55.299999999999855</v>
       </c>
-      <c r="J9" s="14">
-        <f t="shared" ref="J9:J11" si="2">I9/60</f>
+      <c r="J9" s="12">
+        <f t="shared" ref="J9:J14" si="2">I9/60</f>
         <v>0.9216666666666643</v>
       </c>
       <c r="K9" s="3">
@@ -2588,92 +2770,372 @@
         <v>37.997999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:14 3117:3117" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="31" t="s">
+    <row r="10" spans="1:14 3117:3117" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="24">
+        <v>45601</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="3">
+        <v>11005</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.38819444444444445</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0.44108796296296299</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6">
+        <f>(E10-D10)*1440</f>
+        <v>76.166666666666686</v>
+      </c>
+      <c r="J10" s="12">
+        <f t="shared" si="2"/>
+        <v>1.2694444444444448</v>
+      </c>
+      <c r="K10" s="3">
+        <v>25.588000000000001</v>
+      </c>
+      <c r="L10" s="21">
+        <v>99.951999999999998</v>
+      </c>
+      <c r="M10" s="3">
+        <v>4.8255999999999997</v>
+      </c>
+      <c r="N10" s="3">
+        <v>36.921999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14 3117:3117" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="1">
         <v>1500000</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="20">
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="18">
         <v>10</v>
       </c>
-      <c r="G10" s="32">
-        <f t="shared" si="0"/>
+      <c r="G11" s="23">
+        <f>((C11*I5)/C5)</f>
         <v>13973.70500754364</v>
       </c>
-      <c r="H10" s="32">
-        <f>G10/60</f>
+      <c r="H11" s="23">
+        <f>G11/60</f>
         <v>232.89508345906066</v>
       </c>
-      <c r="I10" s="32">
-        <f t="shared" si="1"/>
+      <c r="I11" s="6">
+        <f t="shared" ref="I11" si="3">(E11-D11)*1440</f>
         <v>0</v>
       </c>
-      <c r="J10" s="33">
+      <c r="J11" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K10" s="31"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10"/>
-      <c r="DOW10" t="s">
+      <c r="K11" s="22"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11"/>
+      <c r="DOW11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:14 3117:3117" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="34">
+    <row r="12" spans="1:14 3117:3117" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="24">
         <v>45601</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="3">
-        <v>11005</v>
-      </c>
-      <c r="D11" s="9">
-        <v>0.38819444444444445</v>
-      </c>
-      <c r="E11" s="9">
-        <v>0.44108796296296299</v>
-      </c>
-      <c r="F11" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6">
-        <f>(E11-D11)*1440</f>
-        <v>76.166666666666686</v>
-      </c>
-      <c r="J11" s="14">
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="37">
+        <v>1134626</v>
+      </c>
+      <c r="D12" s="32">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="E12" s="32">
+        <v>0.64444444444444449</v>
+      </c>
+      <c r="F12" s="18">
+        <v>10</v>
+      </c>
+      <c r="G12" s="23">
+        <f>((C12*I5)/C5)</f>
+        <v>10569.952678592806</v>
+      </c>
+      <c r="H12" s="23">
+        <f>G12/60</f>
+        <v>176.16587797654677</v>
+      </c>
+      <c r="I12" s="6">
+        <f>(E12-D12)*1440</f>
+        <v>133</v>
+      </c>
+      <c r="J12" s="12">
         <f t="shared" si="2"/>
-        <v>1.2694444444444448</v>
-      </c>
-      <c r="K11" s="3">
-        <v>25.588000000000001</v>
-      </c>
-      <c r="L11" s="30">
-        <v>99.951999999999998</v>
-      </c>
-      <c r="M11" s="3">
-        <v>4.8255999999999997</v>
-      </c>
-      <c r="N11" s="35">
-        <v>36.921999999999997</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14 3117:3117" x14ac:dyDescent="0.35">
-      <c r="G13" s="10"/>
-    </row>
-    <row r="15" spans="1:14 3117:3117" x14ac:dyDescent="0.35">
-      <c r="C15" s="7"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="13"/>
-    </row>
+        <v>2.2166666666666668</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14 3117:3117" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="24">
+        <v>45601</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1129229</v>
+      </c>
+      <c r="D13" s="32">
+        <v>0.64513888888888893</v>
+      </c>
+      <c r="E13" s="32">
+        <v>0.67638888888888893</v>
+      </c>
+      <c r="F13" s="18">
+        <v>5</v>
+      </c>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23">
+        <f>G13/60</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="6">
+        <f t="shared" ref="I13" si="4">(E13-D13)*1440</f>
+        <v>45</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14 3117:3117" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="24">
+        <v>45601</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1126444</v>
+      </c>
+      <c r="D14" s="32">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="E14" s="32">
+        <v>0.75</v>
+      </c>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23">
+        <f>G14/60</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="6">
+        <f>(E14-D14)*1440</f>
+        <v>104.99999999999994</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="2"/>
+        <v>1.7499999999999991</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14 3117:3117" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="24">
+        <v>45601</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1124220</v>
+      </c>
+      <c r="D15" s="32">
+        <v>0.75</v>
+      </c>
+      <c r="E15" s="32">
+        <v>0.35694444444444445</v>
+      </c>
+      <c r="F15" s="18">
+        <v>8</v>
+      </c>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23">
+        <f>G15/60</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="6">
+        <v>780</v>
+      </c>
+      <c r="J15" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14 3117:3117" ht="40.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="1">
+        <f>C15-C18</f>
+        <v>76836</v>
+      </c>
+      <c r="D16" s="39">
+        <v>45601.75</v>
+      </c>
+      <c r="E16" s="39">
+        <v>45602.356944444444</v>
+      </c>
+      <c r="F16" s="18">
+        <v>8</v>
+      </c>
+      <c r="G16" s="23">
+        <v>780</v>
+      </c>
+      <c r="H16" s="23">
+        <f>G16/60</f>
+        <v>13</v>
+      </c>
+      <c r="I16" s="34"/>
+    </row>
+    <row r="17" spans="1:10" ht="40.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="24"/>
+      <c r="B17" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="1">
+        <v>10043</v>
+      </c>
+      <c r="D17" s="32">
+        <v>0.40972222222222221</v>
+      </c>
+      <c r="E17" s="32">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="F17" s="18">
+        <v>8</v>
+      </c>
+      <c r="G17" s="34">
+        <v>60</v>
+      </c>
+      <c r="H17" s="1">
+        <f>G17/60</f>
+        <v>1</v>
+      </c>
+      <c r="I17" s="34">
+        <v>60</v>
+      </c>
+      <c r="J17" s="1">
+        <f>I17/60</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="24">
+        <v>45602</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1047384</v>
+      </c>
+      <c r="D18" s="32">
+        <v>0.40972222222222221</v>
+      </c>
+      <c r="F18" s="18">
+        <v>8</v>
+      </c>
+      <c r="G18" s="23">
+        <f>((C18*G17)/C17)</f>
+        <v>6257.3971920740814</v>
+      </c>
+      <c r="H18" s="23">
+        <f>G18/60</f>
+        <v>104.2899532012347</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="36">
+        <v>1118478</v>
+      </c>
+      <c r="D19" s="33">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F19" s="18">
+        <v>8</v>
+      </c>
+      <c r="G19" s="23">
+        <f>((C19*G17)/C17)</f>
+        <v>6682.1348202728268</v>
+      </c>
+      <c r="H19" s="23">
+        <f>G19/60</f>
+        <v>111.36891367121378</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1066232</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="35">
+        <f>(H18/24)</f>
+        <v>4.3454147167181123</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="38">
+        <f>(H19/24)</f>
+        <v>4.6403714029672409</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="1">
+        <f>C19-C18</f>
+        <v>71094</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" s="35">
+        <f>G20/2</f>
+        <v>2.1727073583590562</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I21" s="38">
+        <f>I20/2</f>
+        <v>2.3201857014836205</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="1">
+        <f>C12-C19</f>
+        <v>16148</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="H5:H6"/>
@@ -2684,7 +3146,7 @@
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="G5:G6"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -2695,7 +3157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F41588-B940-490C-BA03-A9DB924B9B82}">
   <dimension ref="A1:C356"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A367" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C224" sqref="C224"/>
     </sheetView>
   </sheetViews>
@@ -2726,47 +3188,409 @@
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="224" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C224" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8154D2A-4558-4353-847C-D85F2D5912AF}">
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="40" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="40" style="40"/>
+    <col min="2" max="13" width="18.6328125" style="11" customWidth="1"/>
+    <col min="14" max="16384" width="40" style="40"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="74" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="41">
+        <v>1134626</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0.64444444444444449</v>
+      </c>
+      <c r="E2" s="2">
+        <v>10</v>
+      </c>
+      <c r="F2" s="6">
+        <v>10570</v>
+      </c>
+      <c r="G2" s="6">
+        <f>F2/60</f>
+        <v>176.16666666666666</v>
+      </c>
+      <c r="H2" s="6">
+        <f>(D2-C2)*1440</f>
+        <v>133</v>
+      </c>
+      <c r="I2" s="7">
+        <f t="shared" ref="I2:I7" si="0">H2/60</f>
+        <v>2.2166666666666668</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1129229</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0.64513888888888893</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0.67638888888888893</v>
+      </c>
+      <c r="E3" s="2">
+        <v>5</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6">
+        <f t="shared" ref="G3:G6" si="1">F3/60</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="6">
+        <f t="shared" ref="H3" si="2">(D3-C3)*1440</f>
+        <v>45</v>
+      </c>
+      <c r="I3" s="3">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1126444</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <f>(D4-C4)*1440</f>
+        <v>104.99999999999994</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="0"/>
+        <v>1.7499999999999991</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1124220</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.35694444444444445</v>
+      </c>
+      <c r="E5" s="2">
+        <v>8</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
+        <v>780</v>
+      </c>
+      <c r="I5" s="3">
+        <v>13</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="3">
+        <f>B5-B8</f>
+        <v>76836</v>
+      </c>
+      <c r="C6" s="42">
+        <v>45601.75</v>
+      </c>
+      <c r="D6" s="42">
+        <v>45602.356944444444</v>
+      </c>
+      <c r="E6" s="2">
+        <v>8</v>
+      </c>
+      <c r="F6" s="6">
+        <v>780</v>
+      </c>
+      <c r="G6" s="6">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+    </row>
+    <row r="7" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="3">
+        <v>10043</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.40972222222222221</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="E7" s="2">
+        <v>8</v>
+      </c>
+      <c r="F7" s="6">
+        <v>60</v>
+      </c>
+      <c r="G7" s="3">
+        <f>F7/60</f>
+        <v>1</v>
+      </c>
+      <c r="H7" s="6">
+        <v>60</v>
+      </c>
+      <c r="I7" s="3">
+        <f>H7/60</f>
+        <v>1</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1047384</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.40972222222222221</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="2">
+        <v>8</v>
+      </c>
+      <c r="F8" s="6">
+        <f>((B8*F7)/B7)</f>
+        <v>6257.3971920740814</v>
+      </c>
+      <c r="G8" s="6">
+        <f>F8/60</f>
+        <v>104.2899532012347</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B9" s="21">
+        <v>1118478</v>
+      </c>
+      <c r="C9" s="43">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="2">
+        <v>8</v>
+      </c>
+      <c r="F9" s="6">
+        <f>((B9*F7)/B7)</f>
+        <v>6682.1348202728268</v>
+      </c>
+      <c r="G9" s="6">
+        <f>F9/60</f>
+        <v>111.36891367121378</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+    </row>
+    <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="11">
+        <f>B9-B8</f>
+        <v>71094</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="11">
+        <f>1061933</f>
+        <v>1061933</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="11">
+        <f>B9-B14</f>
+        <v>56545</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="44">
+        <f>(G9/24)</f>
+        <v>4.6403714029672409</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="44">
+        <f>B16/2</f>
+        <v>2.3201857014836205</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
se actualiza documento de evaluación no funcional con el monitoreo de producción para el envío con 10 hilos
</commit_message>
<xml_diff>
--- a/Documento evaluación No Funcional.xlsx
+++ b/Documento evaluación No Funcional.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejandra.ospina\Documents\GitHub\testing-performance-puntos-colombia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38877EB7-B397-4C51-9132-FD080BA9EC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{268069F2-DBCB-410B-B98C-1E6A927FE36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{06B755A2-69F7-43B0-8376-5061E54A97FE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{06B755A2-69F7-43B0-8376-5061E54A97FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Ejecuciones" sheetId="1" r:id="rId1"/>
@@ -90,6 +90,7 @@
     <author>tc={8589356F-B85D-48F5-9A30-671E3104710B}</author>
     <author>tc={BBA738C8-4A2B-4546-8729-695DBFD78E1C}</author>
     <author>tc={FB9D1AF4-0648-4174-BCCD-8D55D0C349C2}</author>
+    <author>tc={4A56A63A-673B-4441-BCF0-222B1229A482}</author>
   </authors>
   <commentList>
     <comment ref="B2" authorId="0" shapeId="0" xr:uid="{FC007BD5-3994-4C6C-BA6A-22C747B225A9}">
@@ -126,12 +127,20 @@
 </t>
       </text>
     </comment>
+    <comment ref="B16" authorId="4" shapeId="0" xr:uid="{4A56A63A-673B-4441-BCF0-222B1229A482}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Dato tomado directamente del Log del micro</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="53">
   <si>
     <t>Prueba</t>
   </si>
@@ -285,15 +294,25 @@
   </si>
   <si>
     <t>Díascon 8 hilos con frecuencia de 30 seg</t>
+  </si>
+  <si>
+    <t>Cantidad de registros procesados en 15 horas con 10 hilos y 30 seg de frecuencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07/11/2024 Despues de la sincronización de las 11 aumentó </t>
+  </si>
+  <si>
+    <t>Díascon 10 hilos con frecuencia de 30 seg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
+    <numFmt numFmtId="177" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -321,7 +340,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -423,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -493,6 +512,45 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -514,43 +572,22 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2344,6 +2381,9 @@
     <text xml:space="preserve">Aumentó después de proceso de sincronización 
 </text>
   </threadedComment>
+  <threadedComment ref="B16" dT="2024-11-07T16:19:30.26" personId="{4E0D853E-4229-4B54-9F3B-11917A4E58D5}" id="{4A56A63A-673B-4441-BCF0-222B1229A482}">
+    <text>Dato tomado directamente del Log del micro</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -2554,10 +2594,10 @@
       <c r="A5" s="13">
         <v>45593</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="40">
         <v>41757</v>
       </c>
       <c r="D5" s="8">
@@ -2566,22 +2606,22 @@
       <c r="E5" s="8">
         <v>0.79166666666666663</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="42">
         <v>4</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="44">
         <f>(C5*I2)/C2</f>
         <v>600.5054285714283</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="38">
         <f>G5/60</f>
         <v>10.008423809523805</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="44">
         <f>((E5-D5)+(E6-D6))*1440</f>
         <v>388.99999999999983</v>
       </c>
-      <c r="J5" s="26">
+      <c r="J5" s="39">
         <f>I5/60</f>
         <v>6.4833333333333307</v>
       </c>
@@ -2602,19 +2642,19 @@
       <c r="A6" s="4">
         <v>45594</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
       <c r="D6" s="8">
         <v>0.29166666666666669</v>
       </c>
       <c r="E6" s="8">
         <v>0.44374999999999998</v>
       </c>
-      <c r="F6" s="30"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="26"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="39"/>
       <c r="K6" s="3">
         <v>1.1598999999999999</v>
       </c>
@@ -2829,11 +2869,11 @@
         <v>13973.70500754364</v>
       </c>
       <c r="H11" s="23">
-        <f>G11/60</f>
+        <f t="shared" ref="H11:H19" si="3">G11/60</f>
         <v>232.89508345906066</v>
       </c>
       <c r="I11" s="6">
-        <f t="shared" ref="I11" si="3">(E11-D11)*1440</f>
+        <f t="shared" ref="I11" si="4">(E11-D11)*1440</f>
         <v>0</v>
       </c>
       <c r="J11" s="12">
@@ -2855,13 +2895,13 @@
       <c r="B12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="37">
+      <c r="C12" s="30">
         <v>1134626</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="25">
         <v>0.55208333333333337</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="25">
         <v>0.64444444444444449</v>
       </c>
       <c r="F12" s="18">
@@ -2872,7 +2912,7 @@
         <v>10569.952678592806</v>
       </c>
       <c r="H12" s="23">
-        <f>G12/60</f>
+        <f t="shared" si="3"/>
         <v>176.16587797654677</v>
       </c>
       <c r="I12" s="6">
@@ -2894,10 +2934,10 @@
       <c r="C13" s="1">
         <v>1129229</v>
       </c>
-      <c r="D13" s="32">
+      <c r="D13" s="25">
         <v>0.64513888888888893</v>
       </c>
-      <c r="E13" s="32">
+      <c r="E13" s="25">
         <v>0.67638888888888893</v>
       </c>
       <c r="F13" s="18">
@@ -2905,11 +2945,11 @@
       </c>
       <c r="G13" s="23"/>
       <c r="H13" s="23">
-        <f>G13/60</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I13" s="6">
-        <f t="shared" ref="I13" si="4">(E13-D13)*1440</f>
+        <f t="shared" ref="I13" si="5">(E13-D13)*1440</f>
         <v>45</v>
       </c>
       <c r="J13" s="1">
@@ -2927,15 +2967,15 @@
       <c r="C14" s="1">
         <v>1126444</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="25">
         <v>0.67708333333333337</v>
       </c>
-      <c r="E14" s="32">
+      <c r="E14" s="25">
         <v>0.75</v>
       </c>
       <c r="G14" s="23"/>
       <c r="H14" s="23">
-        <f>G14/60</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I14" s="6">
@@ -2957,10 +2997,10 @@
       <c r="C15" s="1">
         <v>1124220</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="25">
         <v>0.75</v>
       </c>
-      <c r="E15" s="32">
+      <c r="E15" s="25">
         <v>0.35694444444444445</v>
       </c>
       <c r="F15" s="18">
@@ -2968,7 +3008,7 @@
       </c>
       <c r="G15" s="23"/>
       <c r="H15" s="23">
-        <f>G15/60</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I15" s="6">
@@ -2989,10 +3029,10 @@
         <f>C15-C18</f>
         <v>76836</v>
       </c>
-      <c r="D16" s="39">
+      <c r="D16" s="32">
         <v>45601.75</v>
       </c>
-      <c r="E16" s="39">
+      <c r="E16" s="32">
         <v>45602.356944444444</v>
       </c>
       <c r="F16" s="18">
@@ -3002,10 +3042,10 @@
         <v>780</v>
       </c>
       <c r="H16" s="23">
-        <f>G16/60</f>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="I16" s="34"/>
+      <c r="I16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="40.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="24"/>
@@ -3015,23 +3055,23 @@
       <c r="C17" s="1">
         <v>10043</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="25">
         <v>0.40972222222222221</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="25">
         <v>0.4513888888888889</v>
       </c>
       <c r="F17" s="18">
         <v>8</v>
       </c>
-      <c r="G17" s="34">
+      <c r="G17" s="27">
         <v>60</v>
       </c>
       <c r="H17" s="1">
-        <f>G17/60</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="I17" s="34">
+      <c r="I17" s="27">
         <v>60</v>
       </c>
       <c r="J17" s="1">
@@ -3049,7 +3089,7 @@
       <c r="C18" s="1">
         <v>1047384</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="25">
         <v>0.40972222222222221</v>
       </c>
       <c r="F18" s="18">
@@ -3060,15 +3100,15 @@
         <v>6257.3971920740814</v>
       </c>
       <c r="H18" s="23">
-        <f>G18/60</f>
+        <f t="shared" si="3"/>
         <v>104.2899532012347</v>
       </c>
     </row>
     <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="36">
+      <c r="C19" s="29">
         <v>1118478</v>
       </c>
-      <c r="D19" s="33">
+      <c r="D19" s="26">
         <v>0.45833333333333331</v>
       </c>
       <c r="F19" s="18">
@@ -3079,7 +3119,7 @@
         <v>6682.1348202728268</v>
       </c>
       <c r="H19" s="23">
-        <f>G19/60</f>
+        <f t="shared" si="3"/>
         <v>111.36891367121378</v>
       </c>
     </row>
@@ -3093,14 +3133,14 @@
       <c r="F20" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G20" s="35">
+      <c r="G20" s="28">
         <f>(H18/24)</f>
         <v>4.3454147167181123</v>
       </c>
       <c r="H20" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="I20" s="38">
+      <c r="I20" s="31">
         <f>(H19/24)</f>
         <v>4.6403714029672409</v>
       </c>
@@ -3116,14 +3156,14 @@
       <c r="F21" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="G21" s="35">
+      <c r="G21" s="28">
         <f>G20/2</f>
         <v>2.1727073583590562</v>
       </c>
       <c r="H21" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="I21" s="38">
+      <c r="I21" s="31">
         <f>I20/2</f>
         <v>2.3201857014836205</v>
       </c>
@@ -3235,17 +3275,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8154D2A-4558-4353-847C-D85F2D5912AF}">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="40" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40" style="40"/>
+    <col min="1" max="1" width="40" style="33"/>
     <col min="2" max="13" width="18.6328125" style="11" customWidth="1"/>
-    <col min="14" max="16384" width="40" style="40"/>
+    <col min="14" max="16384" width="40" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="74" customHeight="1" x14ac:dyDescent="0.35">
@@ -3293,7 +3334,7 @@
       <c r="A2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="41">
+      <c r="B2" s="34">
         <v>1134626</v>
       </c>
       <c r="C2" s="8">
@@ -3317,7 +3358,7 @@
         <v>133</v>
       </c>
       <c r="I2" s="7">
-        <f t="shared" ref="I2:I7" si="0">H2/60</f>
+        <f t="shared" ref="I2:I4" si="0">H2/60</f>
         <v>2.2166666666666668</v>
       </c>
       <c r="J2" s="3"/>
@@ -3431,10 +3472,10 @@
         <f>B5-B8</f>
         <v>76836</v>
       </c>
-      <c r="C6" s="42">
+      <c r="C6" s="35">
         <v>45601.75</v>
       </c>
-      <c r="D6" s="42">
+      <c r="D6" s="35">
         <v>45602.356944444444</v>
       </c>
       <c r="E6" s="2">
@@ -3512,20 +3553,26 @@
         <v>104.2899532012347</v>
       </c>
       <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="I8" s="3">
+        <f t="shared" ref="G8:I13" si="3">H8/60</f>
+        <v>0</v>
+      </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="11"/>
       <c r="B9" s="21">
         <v>1118478</v>
       </c>
-      <c r="C9" s="43">
+      <c r="C9" s="36">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="8">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="E9" s="2">
         <v>8</v>
       </c>
@@ -3538,55 +3585,171 @@
         <v>111.36891367121378</v>
       </c>
       <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="I9" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
+    <row r="10" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="3">
+        <v>177684</v>
+      </c>
+      <c r="C10" s="45">
+        <v>45602.729166666664</v>
+      </c>
+      <c r="D10" s="45">
+        <v>45603.351388888892</v>
+      </c>
+      <c r="E10" s="2">
+        <v>10</v>
+      </c>
+      <c r="F10" s="11">
+        <v>1080</v>
+      </c>
+      <c r="G10" s="46">
+        <f>F10/60</f>
+        <v>18</v>
+      </c>
+      <c r="H10" s="11">
+        <v>900</v>
+      </c>
+      <c r="I10" s="3">
+        <f>H10/60</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1059549</v>
+      </c>
+      <c r="C11" s="45">
+        <v>45602.729166666664</v>
+      </c>
+      <c r="E11" s="2">
+        <v>10</v>
+      </c>
+      <c r="F11" s="27">
+        <f>((B11*H10)/B10)</f>
+        <v>5366.7977983386236</v>
+      </c>
+      <c r="G11" s="46">
+        <f>F11/60</f>
+        <v>89.44662997231039</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="3">
+        <v>881467</v>
+      </c>
+      <c r="C12" s="45">
+        <v>45603.354166666664</v>
+      </c>
+      <c r="E12" s="2">
+        <v>10</v>
+      </c>
+      <c r="F12" s="27">
+        <f>((B12*H10)/B10)</f>
+        <v>4464.781859931114</v>
+      </c>
+      <c r="G12" s="46">
+        <f t="shared" si="3"/>
+        <v>74.413030998851895</v>
+      </c>
+    </row>
     <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="47">
+        <v>930890</v>
+      </c>
+      <c r="C13" s="45">
+        <v>45603.459027777775</v>
+      </c>
+      <c r="E13" s="2">
+        <v>10</v>
+      </c>
+      <c r="F13" s="27">
+        <f>((B13*H10)/B10)</f>
+        <v>4715.1178496656985</v>
+      </c>
+      <c r="G13" s="50">
+        <f t="shared" si="3"/>
+        <v>78.585297494428303</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B15" s="11">
         <f>B9-B8</f>
         <v>71094</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
+    <row r="16" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="11">
+        <v>80455</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="11">
-        <f>1061933</f>
-        <v>1061933</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="40" t="s">
+      <c r="B17" s="11">
+        <v>851133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="11">
-        <f>B9-B14</f>
-        <v>56545</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
+      <c r="B18" s="11">
+        <f>B11-B17</f>
+        <v>208416</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="44">
+      <c r="B19" s="37">
         <f>(G9/24)</f>
         <v>4.6403714029672409</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="44">
-        <f>B16/2</f>
+      <c r="B20" s="37">
+        <f>B19/2</f>
         <v>2.3201857014836205</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="49">
+        <f>G13/24</f>
+        <v>3.2743873956011793</v>
       </c>
     </row>
   </sheetData>

</xml_diff>